<commit_message>
Latest with authoring components
</commit_message>
<xml_diff>
--- a/Authoring_TestData.xlsx
+++ b/Authoring_TestData.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="8" r:id="rId1"/>
     <sheet name="Hero" sheetId="1" r:id="rId2"/>
     <sheet name="CTA" sheetId="7" r:id="rId3"/>
-    <sheet name="RTE" sheetId="2" r:id="rId4"/>
-    <sheet name="Accordian" sheetId="3" r:id="rId5"/>
-    <sheet name="ContentCard" sheetId="4" r:id="rId6"/>
-    <sheet name="Header" sheetId="5" r:id="rId7"/>
-    <sheet name="image" sheetId="6" r:id="rId8"/>
+    <sheet name="Headline" sheetId="9" r:id="rId4"/>
+    <sheet name="RTE" sheetId="2" r:id="rId5"/>
+    <sheet name="Accordian" sheetId="3" r:id="rId6"/>
+    <sheet name="ContentCard" sheetId="4" r:id="rId7"/>
+    <sheet name="Header" sheetId="5" r:id="rId8"/>
+    <sheet name="image" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>bgColor</t>
   </si>
@@ -116,19 +117,46 @@
     <t>tests</t>
   </si>
   <si>
-    <t>Hero</t>
-  </si>
-  <si>
     <t>1-2</t>
   </si>
   <si>
     <t>Sample</t>
   </si>
+  <si>
+    <t>headlineText</t>
+  </si>
+  <si>
+    <t>headlineLink</t>
+  </si>
+  <si>
+    <t>headlineLinkOption</t>
+  </si>
+  <si>
+    <t>PlainText</t>
+  </si>
+  <si>
+    <t>Sample Test</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>/content/pathology-education/language-masters/en/testing</t>
+  </si>
+  <si>
+    <t>New tab</t>
+  </si>
+  <si>
+    <t>Existing window/tab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,18 +531,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -522,20 +550,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -552,23 +572,23 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -603,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -638,7 +658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -672,17 +692,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -696,9 +716,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -720,12 +740,59 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -736,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -748,7 +815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -760,7 +827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -772,7 +839,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
authoring component Accordion 7 Image
</commit_message>
<xml_diff>
--- a/Authoring_TestData.xlsx
+++ b/Authoring_TestData.xlsx
@@ -14,13 +14,18 @@
     <sheet name="CTA" sheetId="11" r:id="rId5"/>
     <sheet name="TextBlock" sheetId="13" r:id="rId6"/>
     <sheet name="Carousel" sheetId="14" r:id="rId7"/>
+    <sheet name="PEPList" sheetId="16" r:id="rId8"/>
+    <sheet name="Image" sheetId="19" r:id="rId9"/>
+    <sheet name="Accordion" sheetId="15" r:id="rId10"/>
+    <sheet name="LinkList" sheetId="17" r:id="rId11"/>
+    <sheet name="linkDetails" sheetId="18" r:id="rId12"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="121">
   <si>
     <t>heroText</t>
   </si>
@@ -98,9 +103,6 @@
   </si>
   <si>
     <t>/content/pathology-education/language-masters/en/atlas</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>selectStyle</t>
@@ -227,9 +229,6 @@
     <t>Carousel_Defaultvalues</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>addHeroComponents</t>
   </si>
   <si>
@@ -260,16 +259,166 @@
   </si>
   <si>
     <t>Hero(3,5)</t>
+  </si>
+  <si>
+    <t>transitionDelay</t>
+  </si>
+  <si>
+    <t>pauseOnHoverDisable</t>
+  </si>
+  <si>
+    <t>CHECK</t>
+  </si>
+  <si>
+    <t>UNCHECK</t>
+  </si>
+  <si>
+    <t>Carousel_AutoSlide</t>
+  </si>
+  <si>
+    <t>Carousel_SlideDisabledOnHover</t>
+  </si>
+  <si>
+    <t>expansionType</t>
+  </si>
+  <si>
+    <t>headlines</t>
+  </si>
+  <si>
+    <t>headlineStyle</t>
+  </si>
+  <si>
+    <t>addLinkList</t>
+  </si>
+  <si>
+    <t>textColor</t>
+  </si>
+  <si>
+    <t>bulletIcon</t>
+  </si>
+  <si>
+    <t>textStyle</t>
+  </si>
+  <si>
+    <t>addLinks</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>linkAction</t>
+  </si>
+  <si>
+    <t>OpenStateDefault</t>
+  </si>
+  <si>
+    <t>Default State Open On Page Load</t>
+  </si>
+  <si>
+    <t>Package Inserts
+User Manuals</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>LinkList(1,2)</t>
+  </si>
+  <si>
+    <t>Blue Check</t>
+  </si>
+  <si>
+    <t>linkDetails(1,1)</t>
+  </si>
+  <si>
+    <t>linkDetails(2,6)</t>
+  </si>
+  <si>
+    <t>Instruction For Use</t>
+  </si>
+  <si>
+    <t>https://www.agilent.com/cs/library/packageinsert/public/P03951%20SK006%20NSCLC%20GC%20CC%20UC%20HNSCC%20ESCC%20Rev.%2016.pdf</t>
+  </si>
+  <si>
+    <t>PD-L1 IHC 22C3 pharmDx, Interpretation Manual, Urothelial Carcinoma</t>
+  </si>
+  <si>
+    <t>https://www.agilent.com/cs/library/usermanuals/public/29276_22C3_pharmdx_uc_interpretation_manual_us.pdf</t>
+  </si>
+  <si>
+    <t>PD-L1 IHC 22C3 pharmDx Interpretation Manual, ESCC</t>
+  </si>
+  <si>
+    <t>https://www.agilent.com/cs/library/usermanuals/public/D54358%20rev01%20KN181%20ESCC%20Interpretation%20Manual.pdf</t>
+  </si>
+  <si>
+    <t>PD-L1 IHC 22C3 pharmDx Interpretation Manual, Gastric or GEJ Adenocarcinoma</t>
+  </si>
+  <si>
+    <t>https://www.agilent.com/cs/library/usermanuals/public/29219_pd-l1-ihc-22C3-pharmdx-gastric-interpretation-manual_us.pdf</t>
+  </si>
+  <si>
+    <t>PD-L1 IHC 22C3 pharmDx Interpretation Manual, HNSCC</t>
+  </si>
+  <si>
+    <t>https://www.agilent.com/cs/library/usermanuals/public/29314_22c3_pharmDx_hnscc_interpretation_manual_us.pdf</t>
+  </si>
+  <si>
+    <t>PD-L1 IHC 22C3 pharmDx Interpretation Manual, Cervical Cancer</t>
+  </si>
+  <si>
+    <t>https://www.agilent.com/cs/library/usermanuals/public/29257_22c3_pharmDx_cervical_interpretation_manual_us.pdf</t>
+  </si>
+  <si>
+    <t>Accordion</t>
+  </si>
+  <si>
+    <t>dropImage</t>
+  </si>
+  <si>
+    <t>altText</t>
+  </si>
+  <si>
+    <t>imageCaption</t>
+  </si>
+  <si>
+    <t>captionAsPopup</t>
+  </si>
+  <si>
+    <t>Without Image</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>DefaultValues</t>
+  </si>
+  <si>
+    <t>CaptionAsPopupSelected</t>
+  </si>
+  <si>
+    <t>/content/dam/pathology-education</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -292,10 +441,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -307,8 +457,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -611,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,7 +789,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -651,15 +805,31 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -668,12 +838,208 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="36.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="73" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,7 +1057,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -707,27 +1073,44 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -763,7 +1146,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -771,7 +1154,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -782,7 +1165,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -796,7 +1179,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -805,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -859,35 +1242,35 @@
         <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -902,35 +1285,35 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -945,18 +1328,18 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -971,7 +1354,7 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1003,30 +1386,30 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1034,10 +1417,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1046,30 +1429,30 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
         <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1099,40 +1482,40 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1142,46 +1525,184 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
         <v>62</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
       <c r="D1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PEP List implementation & Code refactoring
</commit_message>
<xml_diff>
--- a/Authoring_TestData.xlsx
+++ b/Authoring_TestData.xlsx
@@ -20,13 +20,14 @@
     <sheet name="linkDetails" sheetId="18" r:id="rId11"/>
     <sheet name="PEPList" sheetId="16" r:id="rId12"/>
     <sheet name="FixedList" sheetId="20" r:id="rId13"/>
+    <sheet name="ChildPages" sheetId="21" r:id="rId14"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="161">
   <si>
     <t>heroText</t>
   </si>
@@ -119,9 +120,6 @@
   </si>
   <si>
     <t>iconPosition</t>
-  </si>
-  <si>
-    <t>buttontextColor</t>
   </si>
   <si>
     <t>View Cource</t>
@@ -274,9 +272,6 @@
     <t>UNCHECK</t>
   </si>
   <si>
-    <t>Carousel_AutoSlide</t>
-  </si>
-  <si>
     <t>Carousel_SlideDisabledOnHover</t>
   </si>
   <si>
@@ -437,12 +432,6 @@
     <t>hideImage</t>
   </si>
   <si>
-    <t>hidePEPDescription</t>
-  </si>
-  <si>
-    <t>hideCategoryTags</t>
-  </si>
-  <si>
     <t>hideEventDate</t>
   </si>
   <si>
@@ -452,24 +441,12 @@
     <t>page</t>
   </si>
   <si>
-    <t>hidePEPImage</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
-    <t>hidePEPDescriptionFixed</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>hidePEPTags</t>
-  </si>
-  <si>
-    <t>categoryTag</t>
-  </si>
-  <si>
     <t>featureFlag</t>
   </si>
   <si>
@@ -479,21 +456,6 @@
     <t>buttonIconPosition</t>
   </si>
   <si>
-    <t>showWebinarProps</t>
-  </si>
-  <si>
-    <t>eventDate</t>
-  </si>
-  <si>
-    <t>eventPresenterName</t>
-  </si>
-  <si>
-    <t>eventPresenterTitle</t>
-  </si>
-  <si>
-    <t>FixedList(1,1)</t>
-  </si>
-  <si>
     <t>Image_DefaultValues</t>
   </si>
   <si>
@@ -510,6 +472,57 @@
   </si>
   <si>
     <t>List_WithFixedList</t>
+  </si>
+  <si>
+    <t>Carousel_SlideEnabledOnHover</t>
+  </si>
+  <si>
+    <t>gridOption</t>
+  </si>
+  <si>
+    <t>showBrandLines</t>
+  </si>
+  <si>
+    <t>/content/pathology-education/language-masters/en/e-learning</t>
+  </si>
+  <si>
+    <t>PEPList</t>
+  </si>
+  <si>
+    <t>/content/pathology-education/language-masters/en/webinars</t>
+  </si>
+  <si>
+    <t>/content/pathology-education/language-masters/en/videos</t>
+  </si>
+  <si>
+    <t>/content/pathology-education/language-masters/en/webinars/library-of-previously-conducted-pd-l1-related-webinars</t>
+  </si>
+  <si>
+    <t>Grid Text</t>
+  </si>
+  <si>
+    <t>3 Column grid</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>FixedList(1,5)</t>
+  </si>
+  <si>
+    <t>AddChildPages</t>
+  </si>
+  <si>
+    <t>ChildPages(1,1)</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>hideDescription</t>
+  </si>
+  <si>
+    <t>hideTags</t>
   </si>
 </sst>
 </file>
@@ -899,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -915,28 +928,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -944,7 +957,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -970,29 +983,29 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
-      </c>
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
         <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1015,37 +1028,37 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1053,21 +1066,21 @@
     </row>
     <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1075,13 +1088,13 @@
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1100,102 +1113,97 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
         <v>119</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>120</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" t="s">
         <v>122</v>
       </c>
-      <c r="F1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M1" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
         <v>155</v>
-      </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1206,15 +1214,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
@@ -1226,37 +1234,32 @@
     <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="G1" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
         <v>18</v>
@@ -1265,25 +1268,91 @@
         <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M1" t="s">
-        <v>146</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>147</v>
       </c>
-      <c r="P1" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="54.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1293,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1317,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1333,28 +1402,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1362,9 +1431,17 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1379,12 +1456,12 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
@@ -1406,7 +1483,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1414,7 +1491,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1425,7 +1502,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -1439,7 +1516,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1448,7 +1525,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1460,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1470,8 +1547,8 @@
     <col min="3" max="3" width="59.81640625" customWidth="1"/>
     <col min="4" max="4" width="39.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1493,10 +1570,10 @@
         <v>16</v>
       </c>
       <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -1507,13 +1584,13 @@
     </row>
     <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1524,13 +1601,13 @@
     </row>
     <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -1539,10 +1616,10 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
       <c r="I3" t="s">
         <v>27</v>
@@ -1550,13 +1627,13 @@
     </row>
     <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1567,13 +1644,13 @@
     </row>
     <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1582,10 +1659,10 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>
@@ -1593,13 +1670,13 @@
     </row>
     <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1608,13 +1685,13 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
       <c r="I6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1624,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1638,10 +1715,9 @@
     <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1660,27 +1736,24 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1689,30 +1762,30 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
@@ -1750,32 +1823,32 @@
     </row>
     <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +1861,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1806,73 +1879,67 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3">
         <v>10000</v>
       </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>10000</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1902,47 +1969,47 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>111</v>
-      </c>
-      <c r="D1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1972,50 +2039,50 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" t="s">
         <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
         <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added video playlist & Video component
</commit_message>
<xml_diff>
--- a/Authoring_TestData.xlsx
+++ b/Authoring_TestData.xlsx
@@ -15,21 +15,22 @@
     <sheet name="TextBlock" sheetId="13" r:id="rId6"/>
     <sheet name="Carousel" sheetId="14" r:id="rId7"/>
     <sheet name="Image" sheetId="19" r:id="rId8"/>
-    <sheet name="Accordion" sheetId="15" r:id="rId9"/>
-    <sheet name="LinkList" sheetId="17" r:id="rId10"/>
-    <sheet name="linkDetails" sheetId="18" r:id="rId11"/>
-    <sheet name="PEPList" sheetId="16" r:id="rId12"/>
-    <sheet name="ChildPages" sheetId="21" r:id="rId13"/>
-    <sheet name="FixedList" sheetId="20" r:id="rId14"/>
-    <sheet name="Webinar" sheetId="22" r:id="rId15"/>
-    <sheet name="CTAButtons" sheetId="23" r:id="rId16"/>
+    <sheet name="Video" sheetId="24" r:id="rId9"/>
+    <sheet name="Accordion" sheetId="15" r:id="rId10"/>
+    <sheet name="LinkList" sheetId="17" r:id="rId11"/>
+    <sheet name="linkDetails" sheetId="18" r:id="rId12"/>
+    <sheet name="PEPList" sheetId="16" r:id="rId13"/>
+    <sheet name="ChildPages" sheetId="21" r:id="rId14"/>
+    <sheet name="FixedList" sheetId="20" r:id="rId15"/>
+    <sheet name="Webinar" sheetId="22" r:id="rId16"/>
+    <sheet name="CTAButtons" sheetId="23" r:id="rId17"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="218">
   <si>
     <t>heroText</t>
   </si>
@@ -545,9 +546,6 @@
     <t>1-6</t>
   </si>
   <si>
-    <t>1-5</t>
-  </si>
-  <si>
     <t>webinarPageSource</t>
   </si>
   <si>
@@ -672,6 +670,33 @@
   </si>
   <si>
     <t>View Webinar</t>
+  </si>
+  <si>
+    <t>List_VideoPalylist</t>
+  </si>
+  <si>
+    <t>Video Playlist</t>
+  </si>
+  <si>
+    <t>FixedList(9,9)</t>
+  </si>
+  <si>
+    <t>/content/pathology-education/language-masters/en/videos/video-full</t>
+  </si>
+  <si>
+    <t>dropVideo</t>
+  </si>
+  <si>
+    <t>dropThumbnail</t>
+  </si>
+  <si>
+    <t>Video_Test</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1037,16 +1062,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
+      <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1111,6 +1136,14 @@
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1120,6 +1153,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1163,7 +1269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1261,12 +1367,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1312,10 +1418,10 @@
         <v>124</v>
       </c>
       <c r="J1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1366,10 +1472,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
         <v>198</v>
-      </c>
-      <c r="B4" t="s">
-        <v>199</v>
       </c>
       <c r="C4" t="s">
         <v>152</v>
@@ -1381,15 +1487,15 @@
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" t="s">
         <v>121</v>
@@ -1398,15 +1504,15 @@
         <v>123</v>
       </c>
       <c r="J5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" t="s">
         <v>181</v>
-      </c>
-      <c r="B6" t="s">
-        <v>182</v>
       </c>
       <c r="E6" t="s">
         <v>121</v>
@@ -1415,10 +1521,27 @@
         <v>123</v>
       </c>
       <c r="J6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K6" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1483,12 +1606,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1512,19 +1635,19 @@
         <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" t="s">
         <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" t="s">
         <v>133</v>
       </c>
       <c r="F1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G1" t="s">
         <v>157</v>
@@ -1572,35 +1695,40 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I9" t="s">
         <v>203</v>
       </c>
-      <c r="I9" t="s">
-        <v>204</v>
-      </c>
       <c r="J9" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -1633,85 +1761,85 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
         <v>168</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>169</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>170</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>171</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>172</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>173</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>174</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>175</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>176</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>177</v>
-      </c>
-      <c r="K1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>185</v>
+      </c>
+      <c r="K4" t="s">
         <v>186</v>
-      </c>
-      <c r="K4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1719,7 +1847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1735,10 +1863,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C1" t="s">
         <v>29</v>
@@ -1749,42 +1877,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1798,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1878,7 +2006,15 @@
         <v>147</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2498,70 +2634,39 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>